<commit_message>
Entrega Final - Laboratorio 5
</commit_message>
<xml_diff>
--- a/Docs/Maquina 1 - Tablas de Datos Lab 4.xlsx
+++ b/Docs/Maquina 1 - Tablas de Datos Lab 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CAMI\EDA\Reto1-G01\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatig\OneDrive\Desktop\EDA\Reto1-G01\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EED33C-8F91-4F90-A694-F8AF237781F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EB0091-F6D0-43E0-90D1-E7A50AACBB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
       <name val="Dax-Regular"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +152,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,11 +176,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -248,20 +263,34 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -309,54 +338,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -514,19 +495,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1261,34 +1229,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>359.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>906.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>180</c:v>
+                  <c:v>1890.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>210</c:v>
+                  <c:v>4546.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>300</c:v>
+                  <c:v>12984.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1390,34 +1352,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>46.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>203.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>906.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>170</c:v>
+                  <c:v>2015.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>190</c:v>
+                  <c:v>4359.375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>210</c:v>
+                  <c:v>9375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>230</c:v>
+                  <c:v>20218.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>250</c:v>
+                  <c:v>30234.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4536,7 +4498,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Datos Lab4-5'!$E$1</c:f>
+              <c:f>'Datos Lab4'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4615,10 +4577,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4642,51 +4604,39 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$E$2:$E$11</c:f>
+              <c:f>'Datos Lab4'!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>359.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>906.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>1890.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>4546.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200</c:v>
+                  <c:v>12984.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4703,7 +4653,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Datos Lab4-5'!$E$14</c:f>
+              <c:f>'Datos Lab4'!$E$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4782,10 +4732,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$15:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4797,63 +4747,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$E$15:$E$24</c:f>
+              <c:f>'Datos Lab4'!$E$15:$E$18</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>2250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>11187.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>50187.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>300</c:v>
+                  <c:v>208062.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5281,7 +5195,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Datos Lab4-5'!$F$1</c:f>
+              <c:f>'Datos Lab4'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5361,7 +5275,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5393,46 +5307,46 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$F$2:$F$11</c:f>
+              <c:f>'Datos Lab4'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>46.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>203.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>906.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>2015.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>4359.375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270</c:v>
+                  <c:v>9375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>300</c:v>
+                  <c:v>20218.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>330</c:v>
+                  <c:v>30234.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5449,7 +5363,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Datos Lab4-5'!$F$14</c:f>
+              <c:f>'Datos Lab4'!$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5529,10 +5443,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$15:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -5550,57 +5464,33 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[1]Datos Lab4-5'!$F$15:$F$24</c:f>
+              <c:f>'Datos Lab4'!$F$15:$F$20</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>343.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>1312.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>5031.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>19765</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>84640.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>250</c:v>
+                  <c:v>348890.625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9896,7 +9786,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9EDF2DAA-D6F8-417C-BFFC-E77C9EABD687}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9907,7 +9797,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:ext cx="9290137" cy="6071644"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9940,7 +9830,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9294395" cy="6075947"/>
+    <xdr:ext cx="9291053" cy="6062579"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10006,7 +9896,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:ext cx="9290137" cy="6071644"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10039,7 +9929,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305192" cy="6069135"/>
+    <xdr:ext cx="9297051" cy="6073205"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10072,7 +9962,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:ext cx="9290137" cy="6071644"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10105,7 +9995,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:ext cx="9290137" cy="6071644"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -10384,6 +10274,11 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10396,24 +10291,24 @@
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{9330A1D0-5BFB-4AF1-A9DA-FA1325F4D7CE}" name="Quick Sort [ms]" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{7A29B3B0-27D3-470C-9562-E4A3931E6F9F}" name="Merge Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9330A1D0-5BFB-4AF1-A9DA-FA1325F4D7CE}" name="Quick Sort [ms]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7A29B3B0-27D3-470C-9562-E4A3931E6F9F}" name="Merge Sort [ms]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A14:F24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{312E8704-8231-410C-8BE3-1789AE129E37}" name="Quick Sort [ms]" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{1AF2196F-A9E6-4A54-A981-EA734D7C884C}" name="Merge Sort [ms]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{312E8704-8231-410C-8BE3-1789AE129E37}" name="Quick Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{1AF2196F-A9E6-4A54-A981-EA734D7C884C}" name="Merge Sort [ms]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10716,23 +10611,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -10745,14 +10640,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -10765,14 +10660,15 @@
       <c r="D2" s="13">
         <v>109.375</v>
       </c>
-      <c r="E2" s="25">
-        <v>30</v>
+      <c r="E2" s="28">
+        <v>31.25</v>
       </c>
-      <c r="F2" s="25">
-        <v>70</v>
+      <c r="F2" s="29">
+        <v>46.88</v>
       </c>
+      <c r="H2" s="29"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -10785,14 +10681,15 @@
       <c r="D3" s="14">
         <v>140.625</v>
       </c>
-      <c r="E3" s="25">
-        <v>60</v>
+      <c r="E3" s="28">
+        <v>93.75</v>
       </c>
-      <c r="F3" s="25">
-        <v>90</v>
+      <c r="F3" s="28">
+        <v>93.75</v>
       </c>
+      <c r="H3" s="28"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
@@ -10805,14 +10702,15 @@
       <c r="D4" s="15">
         <v>375</v>
       </c>
-      <c r="E4" s="25">
-        <v>90</v>
+      <c r="E4" s="28">
+        <v>187.5</v>
       </c>
-      <c r="F4" s="25">
-        <v>110</v>
+      <c r="F4" s="29">
+        <v>203.125</v>
       </c>
+      <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
@@ -10825,14 +10723,15 @@
       <c r="D5" s="14">
         <v>593.75</v>
       </c>
-      <c r="E5" s="25">
-        <v>120</v>
+      <c r="E5" s="28">
+        <v>359.375</v>
       </c>
-      <c r="F5" s="25">
-        <v>130</v>
+      <c r="F5" s="28">
+        <v>406.25</v>
       </c>
+      <c r="H5" s="28"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
@@ -10845,14 +10744,15 @@
       <c r="D6" s="15">
         <v>1234.375</v>
       </c>
-      <c r="E6" s="25">
-        <v>150</v>
+      <c r="E6" s="28">
+        <v>906.25</v>
       </c>
-      <c r="F6" s="25">
-        <v>150</v>
+      <c r="F6" s="29">
+        <v>906.25</v>
       </c>
+      <c r="H6" s="29"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
@@ -10861,14 +10761,15 @@
       <c r="D7" s="14">
         <v>2640.625</v>
       </c>
-      <c r="E7" s="25">
-        <v>180</v>
+      <c r="E7" s="28">
+        <v>1890.625</v>
       </c>
-      <c r="F7" s="25">
-        <v>170</v>
+      <c r="F7" s="28">
+        <v>2015.625</v>
       </c>
+      <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
@@ -10877,14 +10778,15 @@
       <c r="D8" s="15">
         <v>7781.25</v>
       </c>
-      <c r="E8" s="25">
-        <v>210</v>
+      <c r="E8" s="28">
+        <v>4546.875</v>
       </c>
-      <c r="F8" s="25">
-        <v>190</v>
+      <c r="F8" s="29">
+        <v>4359.375</v>
       </c>
+      <c r="H8" s="29"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
@@ -10893,14 +10795,15 @@
       <c r="D9" s="14">
         <v>14875</v>
       </c>
-      <c r="E9" s="25">
-        <v>240</v>
+      <c r="E9" s="28">
+        <v>12984.375</v>
       </c>
-      <c r="F9" s="25">
-        <v>210</v>
+      <c r="F9" s="28">
+        <v>9375</v>
       </c>
+      <c r="H9" s="28"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
@@ -10909,14 +10812,13 @@
       <c r="D10" s="15">
         <v>36953.125</v>
       </c>
-      <c r="E10" s="25">
-        <v>270</v>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29">
+        <v>20218.75</v>
       </c>
-      <c r="F10" s="25">
-        <v>230</v>
-      </c>
+      <c r="H10" s="29"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>375942</v>
       </c>
@@ -10925,14 +10827,13 @@
       <c r="D11" s="14">
         <v>65953.125</v>
       </c>
-      <c r="E11" s="25">
-        <v>300</v>
+      <c r="E11" s="28"/>
+      <c r="F11" s="30">
+        <v>30234.375</v>
       </c>
-      <c r="F11" s="25">
-        <v>250</v>
-      </c>
+      <c r="H11" s="30"/>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -10945,14 +10846,14 @@
       <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
@@ -10966,13 +10867,14 @@
         <v>2140.625</v>
       </c>
       <c r="E15" s="27">
-        <v>30</v>
+        <v>2250</v>
       </c>
-      <c r="F15" s="27">
-        <v>70</v>
+      <c r="F15" s="31">
+        <v>343.75</v>
       </c>
+      <c r="H15" s="31"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -10986,13 +10888,14 @@
         <v>8781.25</v>
       </c>
       <c r="E16" s="27">
-        <v>60</v>
+        <v>11187.5</v>
       </c>
       <c r="F16" s="27">
-        <v>90</v>
+        <v>1312.5</v>
       </c>
+      <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
@@ -11002,13 +10905,14 @@
         <v>44734.375</v>
       </c>
       <c r="E17" s="27">
-        <v>90</v>
+        <v>50187.5</v>
       </c>
-      <c r="F17" s="27">
-        <v>110</v>
+      <c r="F17" s="31">
+        <v>5031.25</v>
       </c>
+      <c r="H17" s="31"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
@@ -11018,95 +10922,78 @@
         <v>212031.25</v>
       </c>
       <c r="E18" s="27">
-        <v>120</v>
+        <v>208062.5</v>
       </c>
       <c r="F18" s="27">
-        <v>130</v>
+        <v>19765</v>
       </c>
+      <c r="H18" s="27"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="27">
-        <v>150</v>
+      <c r="E19" s="27"/>
+      <c r="F19" s="31">
+        <v>84640.625</v>
       </c>
-      <c r="F19" s="27">
-        <v>150</v>
-      </c>
+      <c r="H19" s="31"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="27">
-        <v>180</v>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27">
+        <v>348890.625</v>
       </c>
-      <c r="F20" s="27">
-        <v>170</v>
-      </c>
+      <c r="H20" s="27"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="27">
-        <v>210</v>
-      </c>
-      <c r="F21" s="27">
-        <v>190</v>
-      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="27">
-        <v>240</v>
-      </c>
-      <c r="F22" s="27">
-        <v>210</v>
-      </c>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="27">
-        <v>270</v>
-      </c>
-      <c r="F23" s="27">
-        <v>230</v>
-      </c>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>375942</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="21"/>
-      <c r="E24" s="27">
-        <v>300</v>
-      </c>
-      <c r="F24" s="27">
-        <v>250</v>
-      </c>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11118,6 +11005,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c10596efcc8303131ba000bf7988b65d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88645b4f568d2e9f6d2a1da3b5a5f323" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -11328,12 +11221,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11344,6 +11231,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21480DE1-6D35-4CDC-8EE6-012EAA9B4D3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11362,23 +11266,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>

</xml_diff>